<commit_message>
Update DB (Add Tarushi)
</commit_message>
<xml_diff>
--- a/backend/data/hci_data.xlsx
+++ b/backend/data/hci_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13df6996760a0db9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9320EC5E-1E9A-4D1D-9526-C80FD6CC5069}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2C2CC95-5824-4540-8D09-5A4D62342013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="890" yWindow="-110" windowWidth="18420" windowHeight="11020" firstSheet="2" activeTab="2" xr2:uid="{0152CC16-2486-4035-A65F-2AD5729C8634}"/>
+    <workbookView xWindow="890" yWindow="-110" windowWidth="18420" windowHeight="11020" firstSheet="4" activeTab="5" xr2:uid="{0152CC16-2486-4035-A65F-2AD5729C8634}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="376">
   <si>
     <t>ID</t>
   </si>
@@ -340,6 +340,46 @@
     <t>Machine Learning</t>
   </si>
   <si>
+    <t>WGS7500</t>
+  </si>
+  <si>
+    <t>cf6d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This course is a graduate-only advanced introduction (inevitably partial and selective) to key concepts, thinkers, and texts in the fields of feminist and queer theory. The goal is to develop a foundation for your own research and teaching on gender and sexuality. Together, we will explore books and articles that have traveled across disciplines to shape debate in a variety of fields.
+</t>
+  </si>
+  <si>
+    <t>https://applications.zoom.us/lti/rich/j/98002680351?oauth_consumer_key=WtcHJWd4RR6b7CXImqvBxQ&amp;lti_scid=25853fb1d39a813262709ed907bd631b22dea25c18c07a0647f423a699705c88</t>
+  </si>
+  <si>
+    <t>Approaches to Gender and Sexuality Studies</t>
+  </si>
+  <si>
+    <t>DEM7000</t>
+  </si>
+  <si>
+    <t>jes4fx</t>
+  </si>
+  <si>
+    <t>https://applications.zoom.us/lti/rich/j/99708580643?oauth_consumer_key=WtcHJWd4RR6b7CXImqvBxQ&amp;lti_scid=cf287ae43f7676443aefd78c74a9ca53e03ed16fc07b0e702839eefea7125bd2</t>
+  </si>
+  <si>
+    <t>War, Violence and Democracy</t>
+  </si>
+  <si>
+    <t>ENGL8578</t>
+  </si>
+  <si>
+    <t>acb2hf</t>
+  </si>
+  <si>
+    <t>http://gmail.com/</t>
+  </si>
+  <si>
+    <t>Literature of the Americas</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
@@ -563,6 +603,15 @@
   </si>
   <si>
     <t>https://calendar.google.com/calendar/embed?src=YmJycHY4YmUxcTYxMWV0NzVyb2J2OWtjamdAZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;src=MDhhdWs3aTFrOWxxcmJsMTlwYTdsYmw0dDBAZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;color=%23009688&amp;color=%23F4511E</t>
+  </si>
+  <si>
+    <t>Tarushi</t>
+  </si>
+  <si>
+    <t>12,13,14</t>
+  </si>
+  <si>
+    <t>https://calendar.google.com/calendar/embed?src=czkwNzJsOHZwYWk0Zjk1dGFzcXMwMDQ3N2tAZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;src=MWZhYjFjZzRsMzg2Y2xpZ2M4M3ZuYmNoMGtAZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;src=OHZrYWc5aHRoMDIzb2FlNXNvaHB0YTZ1bm9AZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;color=%23F4511E&amp;color=%23795548&amp;color=%23F09300</t>
   </si>
   <si>
     <t>AssignmentID</t>
@@ -911,6 +960,46 @@
   </si>
   <si>
     <t>https://collab.its.virginia.edu/portal/directtool/7c8b6b9c-aa69-4e8b-8832-68ed6c0276b6/</t>
+  </si>
+  <si>
+    <t>Draft Syllabus</t>
+  </si>
+  <si>
+    <t>We will workshop these drafts in class. 
+Your draft syllabus should include the following elements: 
+            Course Description
+            Learning Objectives
+            Materials
+Class expectations
+Assignments (you must include one essay assignment)
+            Assessment Information (what rubric will you use)
+            Schedule for a twelve-week semester.
+The schedule should include specific reading, writing, listening, or watching assignments</t>
+  </si>
+  <si>
+    <t>Nov 17, 2020 1:00 pm</t>
+  </si>
+  <si>
+    <t>https://collab.its.virginia.edu/portal/site/13d4af25-0367-4078-9318-fbbbe0033f2e/tool/5f3ce9b5-503a-4f54-a034-3717c814d97c?panel=Main</t>
+  </si>
+  <si>
+    <t>Final Syllabus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your final assignment is to produce a complete syllabus for a twelve-week undergraduate seminar or lecture course focused on gender and/or sexuality.  This is an opportunity to build a class for your teaching portfolio and to think about feminist and queer approaches to pedagogy.  What readings would you teach?  How would you organize them?  What assignments would you use to engage students with readings?
+</t>
+  </si>
+  <si>
+    <t>Nov 24, 2020 11:00 pm</t>
+  </si>
+  <si>
+    <t>Review Essay</t>
+  </si>
+  <si>
+    <t>A reflection review essay of things read this week</t>
+  </si>
+  <si>
+    <t>Nov 18, 2020 11:59 pm</t>
   </si>
   <si>
     <t>Date</t>
@@ -1122,6 +1211,27 @@
   </si>
   <si>
     <t>Nov 16, 2020 9:59 pm</t>
+  </si>
+  <si>
+    <t>Environmentalism, Fantasy and Intersectionality A Comparison Between the US and the EU | November 5-6, 2020</t>
+  </si>
+  <si>
+    <t>Nov 4, 2020 2:04 pm</t>
+  </si>
+  <si>
+    <t>https://jmce.unc.edu/environmentalism-fantasy-intersectionality/</t>
+  </si>
+  <si>
+    <t>Into the Desert: Questions of Coloniality and Toxicity Lecture Series</t>
+  </si>
+  <si>
+    <t>I just came across an announcement for this series of lectures on deserts as spaces of colonialism and toxicity, which is being coordinated by one of our guests for this semester, architecture historian Samia Henni. It looks like the speakers will touch on issues of interest to many of you.</t>
+  </si>
+  <si>
+    <t>Sep 22, 2020 10:57 am</t>
+  </si>
+  <si>
+    <t>https://aap.cornell.edu/news-events/desert-questions-coloniality-and-toxicity</t>
   </si>
 </sst>
 </file>
@@ -1548,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3D680F-EDDF-4B08-83B1-9E2B212E0B07}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1962,6 +2072,60 @@
       </c>
       <c r="K12" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2016,9 +2180,12 @@
     <hyperlink ref="F12" r:id="rId48" xr:uid="{518389A0-EB17-4819-B4FC-57356885DB27}"/>
     <hyperlink ref="G2" r:id="rId49" xr:uid="{C558F49D-7D66-4960-B3DF-187CAB77FEED}"/>
     <hyperlink ref="H2" r:id="rId50" xr:uid="{0B536188-2E7F-4C0A-80B8-186C311568FC}"/>
+    <hyperlink ref="F13" r:id="rId51" xr:uid="{C8EAE357-DC64-46E8-8667-0379E8F2D90A}"/>
+    <hyperlink ref="F14" r:id="rId52" xr:uid="{FE031A48-8E5A-4BFD-84DE-83A5CBCB633A}"/>
+    <hyperlink ref="F15" r:id="rId53" xr:uid="{C2F5C900-893F-45A0-881F-76AAB8C4D494}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId51"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 
@@ -2037,135 +2204,135 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15">
       <c r="A10" s="11" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2177,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A567B86-7532-44B8-953F-0EDE11A50FFA}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2188,227 +2355,240 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="15">
       <c r="A10" s="15" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="C10" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="C15" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="17" ht="15"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15">
+      <c r="A17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{84AB97E5-8A67-4633-9DEB-06CF5FD2600D}"/>
@@ -2426,6 +2606,7 @@
     <hyperlink ref="D12" r:id="rId13" display="https://calendar.google.com/calendar/embed?src=dGRuYnBuY3VqMmxmY2ZsNXN1NHVrZWoyZ2NAZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;src=Mzd0c2M0MGxwbXFjdG1uNTUwOWsyZW5oMGNAZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;src=MjJlaml1aXF0dGZlbnV1a2pwbDBkaWdnYWtAZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;color=%23F4511E&amp;color=%233F51B5&amp;color=%238E24AA" xr:uid="{5B0EECA7-8056-4C9F-BAA9-42D011B492AB}"/>
     <hyperlink ref="D9" r:id="rId14" xr:uid="{5A9E948E-423C-4854-BFE2-D5E98398B590}"/>
     <hyperlink ref="D13" r:id="rId15" display="https://calendar.google.com/calendar/embed?src=aDkxczdicGJraTNldDcyYTFhZjU4cDlhZ29AZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;src=Y3UxMnNnYWZyMmtqanFhbnE4N2U1Mjhpbm9AZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;src=dGlpa3NpazJxazh2ZjE0N2pucjJ1dG9sOW9AZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;color=%23C0CA33&amp;color=%23B39DDB&amp;color=%23E67C73" xr:uid="{042FF906-6ADB-49E6-AE34-99F3F3B59B8B}"/>
+    <hyperlink ref="D17" r:id="rId16" display="https://calendar.google.com/calendar/embed?src=czkwNzJsOHZwYWk0Zjk1dGFzcXMwMDQ3N2tAZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;src=MWZhYjFjZzRsMzg2Y2xpZ2M4M3ZuYmNoMGtAZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;src=OHZrYWc5aHRoMDIzb2FlNXNvaHB0YTZ1bm9AZ3JvdXAuY2FsZW5kYXIuZ29vZ2xlLmNvbQ&amp;color=%23F4511E&amp;color=%23795548&amp;color=%23F09300" xr:uid="{7351A6EF-467A-44D6-ABDA-C14211B505D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2435,8 +2616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21BA0A2-F4EC-4668-A98E-245E730439B9}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2450,13 +2631,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -2474,10 +2655,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2488,10 +2669,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -2508,10 +2689,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -2528,10 +2709,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -2548,10 +2729,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -2568,10 +2749,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2588,10 +2769,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -2608,10 +2789,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -2628,10 +2809,10 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2642,10 +2823,10 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2656,10 +2837,10 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2670,10 +2851,10 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2684,10 +2865,10 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2698,10 +2879,10 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2712,10 +2893,10 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2726,10 +2907,10 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2740,10 +2921,10 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2754,10 +2935,10 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2768,10 +2949,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2782,10 +2963,10 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2796,10 +2977,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2810,10 +2991,10 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2824,10 +3005,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2838,10 +3019,10 @@
         <v>22</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2877,10 +3058,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFF53B4-FACD-4A05-8D76-7FD0BDBEA621}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2897,25 +3078,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2926,19 +3107,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -2950,19 +3131,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="D3" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2973,22 +3154,22 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
@@ -2999,22 +3180,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="F5">
         <v>100</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15">
@@ -3025,22 +3206,22 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="D6" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="F6">
         <v>100</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15">
@@ -3051,19 +3232,19 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="F7">
         <v>100</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15">
@@ -3074,19 +3255,19 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="D8" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="F8">
         <v>100</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15">
@@ -3097,19 +3278,19 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="F9">
         <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15">
@@ -3120,19 +3301,19 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="D10" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="F10">
         <v>4</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15">
@@ -3143,19 +3324,19 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15">
@@ -3166,19 +3347,19 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15">
@@ -3189,19 +3370,19 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="D13" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="F13">
         <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15">
@@ -3212,19 +3393,19 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="D14" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="F14">
         <v>10</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15">
@@ -3235,19 +3416,19 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="D15" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="F15">
         <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15">
@@ -3258,19 +3439,19 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="D16" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="F16">
         <v>10</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15">
@@ -3281,19 +3462,19 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="D17" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="F17">
         <v>10</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15">
@@ -3304,16 +3485,16 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="F18">
         <v>25</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15">
@@ -3324,19 +3505,19 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="D19" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="F19">
         <v>600</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15">
@@ -3347,19 +3528,19 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="F20" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15">
@@ -3370,19 +3551,19 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="D21" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="F21" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>208</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15">
@@ -3393,22 +3574,90 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="D22" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="F22">
         <v>125</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>301</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="F23" t="s">
+        <v>296</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>305</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F24" t="s">
+        <v>296</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>308</v>
+      </c>
+      <c r="D25" t="s">
+        <v>309</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="F25" t="s">
+        <v>296</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{04A7ADE2-A754-4A93-9957-02FD7B22ED8A}"/>
@@ -3435,6 +3684,9 @@
     <hyperlink ref="G15" r:id="rId22" xr:uid="{134B7431-02F7-4FAB-9931-0B36B311DE6B}"/>
     <hyperlink ref="G21" r:id="rId23" xr:uid="{B608D92D-1F58-4A39-AD07-89569697B0DC}"/>
     <hyperlink ref="G22" r:id="rId24" xr:uid="{C70AD4D4-33D1-4EBB-9439-025B64D113BB}"/>
+    <hyperlink ref="G23" r:id="rId25" xr:uid="{EB65579B-76B8-4600-AFAD-CEC3D8E86D44}"/>
+    <hyperlink ref="G24" r:id="rId26" xr:uid="{8330FFB3-3F13-4839-B929-04790512F2F1}"/>
+    <hyperlink ref="G25" r:id="rId27" xr:uid="{8CD15789-B8C1-414A-9266-6C2495E3669F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3442,10 +3694,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87DF9F39-3440-49F6-B718-A308EB0F14AF}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3458,19 +3710,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>285</v>
+        <v>311</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3481,16 +3733,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>289</v>
+        <v>315</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3501,16 +3753,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>292</v>
+        <v>318</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>293</v>
+        <v>319</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3521,16 +3773,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>295</v>
+        <v>321</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15">
@@ -3541,16 +3793,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>297</v>
+        <v>323</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>298</v>
+        <v>324</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>299</v>
+        <v>325</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15">
@@ -3561,16 +3813,16 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>301</v>
+        <v>327</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>302</v>
+        <v>328</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>303</v>
+        <v>329</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15">
@@ -3581,16 +3833,16 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>304</v>
+        <v>330</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>305</v>
+        <v>331</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15">
@@ -3601,16 +3853,16 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>307</v>
+        <v>333</v>
       </c>
       <c r="D8" t="s">
-        <v>308</v>
+        <v>334</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>309</v>
+        <v>335</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>310</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15">
@@ -3621,16 +3873,16 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>311</v>
+        <v>337</v>
       </c>
       <c r="D9" t="s">
-        <v>312</v>
+        <v>338</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>313</v>
+        <v>339</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>310</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15">
@@ -3641,16 +3893,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>314</v>
+        <v>340</v>
       </c>
       <c r="D10" t="s">
-        <v>315</v>
+        <v>341</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>310</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15">
@@ -3661,16 +3913,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>317</v>
+        <v>343</v>
       </c>
       <c r="D11" t="s">
-        <v>318</v>
+        <v>344</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>320</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15">
@@ -3681,16 +3933,16 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>321</v>
+        <v>347</v>
       </c>
       <c r="D12" t="s">
-        <v>322</v>
+        <v>348</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>320</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15">
@@ -3701,16 +3953,16 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="D13" t="s">
-        <v>325</v>
+        <v>351</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>320</v>
+        <v>346</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15">
@@ -3721,16 +3973,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="D14" t="s">
-        <v>328</v>
+        <v>354</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>330</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -3741,16 +3993,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>331</v>
+        <v>357</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>332</v>
+        <v>358</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>333</v>
+        <v>359</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>334</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15">
@@ -3761,16 +4013,16 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>335</v>
+        <v>361</v>
       </c>
       <c r="D16" t="s">
-        <v>336</v>
+        <v>362</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>337</v>
+        <v>363</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15">
@@ -3781,16 +4033,16 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>338</v>
+        <v>364</v>
       </c>
       <c r="D17" t="s">
-        <v>339</v>
+        <v>365</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>340</v>
+        <v>366</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15">
@@ -3801,16 +4053,53 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>338</v>
+        <v>364</v>
       </c>
       <c r="D18" t="s">
-        <v>341</v>
+        <v>367</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>342</v>
+        <v>368</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>252</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>369</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>372</v>
+      </c>
+      <c r="D20" t="s">
+        <v>373</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3832,6 +4121,8 @@
     <hyperlink ref="F16" r:id="rId15" xr:uid="{4A6877E1-A77A-49CB-8964-4CED7798C598}"/>
     <hyperlink ref="F17" r:id="rId16" xr:uid="{1C4B0FF0-D4E2-469B-B996-DC3C038E2348}"/>
     <hyperlink ref="F18" r:id="rId17" xr:uid="{189B199D-13CD-4473-A805-6480FB0EF04E}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{1E10F744-7A09-49AD-B5D3-837A14206C17}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{542FB6FE-9612-4CC8-8B05-AE9E1FA892E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>